<commit_message>
Created a single SQL script for every developer to avoid each developer creating own database without standard. Please use Overall.sql.
</commit_message>
<xml_diff>
--- a/SQLScripts/BeansLeaveAppTableStructuresV2.xlsx
+++ b/SQLScripts/BeansLeaveAppTableStructuresV2.xlsx
@@ -5,28 +5,27 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="LeaveType" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="LeaveTransaction" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="LeaveAttachment" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="SystemAuditTrail" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="LeaveTransactionAuditTrail" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="EmployeeGrade" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Address" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Department" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="EmployeeType" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="EmployeeProfile" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="YearlyEntitlement" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="AddressType" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="EmployeeGrade" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Address" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Department" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="EmployeeType" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="EmployeeProfile" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="YearlyEntitlement" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="AddressType" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="81">
   <si>
     <t>Field Name</t>
   </si>
@@ -64,13 +63,13 @@
     <t>Description of the particular leave type</t>
   </si>
   <si>
-    <t>empGrade</t>
+    <t>empType</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>Employee Grade</t>
+    <t>Employee Type</t>
   </si>
   <si>
     <t>entitlement</t>
@@ -190,6 +189,9 @@
     <t>postcode</t>
   </si>
   <si>
+    <t>VAR</t>
+  </si>
+  <si>
     <t>employeeNumber</t>
   </si>
   <si>
@@ -199,10 +201,7 @@
     <t>idNumber</t>
   </si>
   <si>
-    <t>idType</t>
-  </si>
-  <si>
-    <t>IC or Passport</t>
+    <t>passportNumber</t>
   </si>
   <si>
     <t>gender</t>
@@ -380,7 +379,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -398,10 +397,6 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -492,13 +487,13 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B44" activeCellId="0" pane="topLeft" sqref="B44"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100">
+      <selection activeCell="D7" activeCellId="0" pane="topLeft" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.9948979591837"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.8265306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.8265306122449"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="33.1632653061224"/>
@@ -567,7 +562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -610,10 +605,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="n">
@@ -639,26 +634,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D19" activeCellId="0" pane="topLeft" sqref="D19"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100">
+      <selection activeCell="D17" activeCellId="0" pane="topLeft" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7295918367347"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
-      <c r="A1" s="0"/>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="2">
       <c r="A2" s="2" t="s">
@@ -684,300 +675,80 @@
       <c r="C3" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
       <c r="A4" s="3" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="5">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>50</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
-      <c r="A6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3"/>
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7">
       <c r="A7" s="4" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
-      <c r="A8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9">
-      <c r="A9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="10">
-      <c r="A10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="11">
-      <c r="A11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="12">
-      <c r="A12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="3" t="n">
-        <v>50</v>
-      </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="13">
-      <c r="A13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>50</v>
-      </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="14">
-      <c r="A14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="15">
-      <c r="A15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="16">
-      <c r="A16" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="17">
-      <c r="A17" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="7"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="18">
-      <c r="A18" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="7"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="19">
-      <c r="A19" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="20">
-      <c r="A20" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="21">
-      <c r="A21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D21" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="22">
-      <c r="A22" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="23">
-      <c r="A23" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="24">
-      <c r="A24" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="25">
-      <c r="A25" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="26">
-      <c r="A26" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="27">
-      <c r="A27" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="3"/>
+      <c r="C8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -990,137 +761,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N50" activeCellId="0" pane="topLeft" sqref="N50"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7295918367347"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
-      <c r="A4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="5">
-      <c r="A5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7">
-      <c r="A7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
-      <c r="A8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N48" activeCellId="0" pane="topLeft" sqref="N48"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100">
+      <selection activeCell="B16" activeCellId="0" pane="topLeft" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1181,10 +825,10 @@
       <c r="D5" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="n">
@@ -1212,7 +856,7 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100">
       <selection activeCell="D18" activeCellId="0" pane="topLeft" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1372,10 +1016,10 @@
       <c r="D13" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="3" t="n">
@@ -1401,7 +1045,7 @@
   </sheetPr>
   <dimension ref="A2:D7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100">
       <selection activeCell="E27" activeCellId="0" pane="topLeft" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -1481,10 +1125,10 @@
       <c r="D6" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="3" t="n">
@@ -1512,8 +1156,8 @@
   </sheetPr>
   <dimension ref="A2:D8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C8" activeCellId="0" pane="topLeft" sqref="C8"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100">
+      <selection activeCell="B20" activeCellId="0" pane="topLeft" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1578,7 +1222,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1590,7 +1234,7 @@
       <c r="D6" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1602,10 +1246,10 @@
       <c r="D7" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="3" t="n">
@@ -1631,128 +1275,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A8" activeCellId="0" pane="topLeft" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
-      <c r="A4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
-      <c r="A5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>50</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
-      <c r="A7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
-      <c r="A8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100">
       <selection activeCell="D14" activeCellId="0" pane="topLeft" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1824,10 +1349,10 @@
       <c r="D5" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="n">
@@ -1835,6 +1360,347 @@
       </c>
       <c r="D6" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q58"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100">
+      <selection activeCell="F16" activeCellId="0" pane="topLeft" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.2142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.8265306122449"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
+      <c r="A1" s="0"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="Q1" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
+      <c r="A4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="5">
+      <c r="A5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q5" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
+      <c r="A6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="Q6" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7">
+      <c r="A7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="Q7" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
+      <c r="A8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="Q8" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9">
+      <c r="A9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="Q9" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="10">
+      <c r="A10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="Q10" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="11">
+      <c r="A11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="Q11" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="12">
+      <c r="A12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="Q12" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="13">
+      <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="14">
+      <c r="Q14" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="15">
+      <c r="Q15" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="16">
+      <c r="Q16" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="17">
+      <c r="Q17" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="18">
+      <c r="Q18" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="19">
+      <c r="Q19" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="20">
+      <c r="Q20" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="21">
+      <c r="Q21" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="22">
+      <c r="Q22" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="23">
+      <c r="Q23" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="24">
+      <c r="Q24" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="25">
+      <c r="Q25" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="26">
+      <c r="Q26" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="27">
+      <c r="Q27" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="28">
+      <c r="Q28" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="29">
+      <c r="Q29" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="30">
+      <c r="Q30" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="31">
+      <c r="Q31" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="32">
+      <c r="Q32" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="33">
+      <c r="Q33" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="34">
+      <c r="Q34" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="35">
+      <c r="Q35" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="36">
+      <c r="Q36" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="37">
+      <c r="Q37" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="38">
+      <c r="Q38" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
+      <c r="Q39" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
+      <c r="Q40" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="41">
+      <c r="Q41" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="42">
+      <c r="Q42" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="43">
+      <c r="Q43" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="44">
+      <c r="Q44" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="45">
+      <c r="Q45" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="46">
+      <c r="Q46" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
+      <c r="Q47" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
+      <c r="Q48" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
+      <c r="Q49" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="50">
+      <c r="Q50" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="51">
+      <c r="Q51" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="52">
+      <c r="Q52" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="53">
+      <c r="Q53" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="54">
+      <c r="Q54" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="55">
+      <c r="Q55" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="56">
+      <c r="Q56" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="57">
+      <c r="Q57" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="58">
+      <c r="Q58" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1853,201 +1719,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="Q58" activeCellId="0" pane="topLeft" sqref="Q58"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.8265306122449"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
-      <c r="A1" s="0"/>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
-      <c r="A4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="5">
-      <c r="A5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
-      <c r="A6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7">
-      <c r="A7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
-      <c r="A8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9">
-      <c r="A9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="10">
-      <c r="A10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="11">
-      <c r="A11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="12">
-      <c r="A12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="13">
-      <c r="A13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100">
+      <selection activeCell="C20" activeCellId="0" pane="topLeft" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -2118,10 +1793,10 @@
       <c r="D5" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="n">
@@ -2142,14 +1817,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100">
       <selection activeCell="H22" activeCellId="0" pane="topLeft" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -2221,10 +1896,10 @@
       <c r="D5" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="n">
@@ -2243,4 +1918,353 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100">
+      <selection activeCell="D9" activeCellId="0" pane="topLeft" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.8265306122449"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
+      <c r="A1" s="0"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
+      <c r="A4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="5">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
+      <c r="A6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7">
+      <c r="A7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+      <c r="A8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9">
+      <c r="A9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="10">
+      <c r="A10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="11">
+      <c r="A11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="12">
+      <c r="A12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="13">
+      <c r="A13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="14">
+      <c r="A14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="15">
+      <c r="A15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="16">
+      <c r="A16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="17">
+      <c r="A17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="18">
+      <c r="A18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="19">
+      <c r="A19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="20">
+      <c r="A20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="21">
+      <c r="A21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="22">
+      <c r="A22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="23">
+      <c r="A23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="24">
+      <c r="A24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="25">
+      <c r="A25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="26">
+      <c r="A26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="27">
+      <c r="A27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>